<commit_message>
some updates in the wireframes
</commit_message>
<xml_diff>
--- a/User Stories/Backlog v2.xlsx
+++ b/User Stories/Backlog v2.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Desktop\TP\ProjetoIntegrado\User Stories\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\joaop\OneDrive\Ambiente de Trabalho\Projeto Integrado\User Stories\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE914B8E-FC9F-41AA-B211-E5DD3A67874D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3609CAC9-5B8D-4AED-A8B4-8C9B2069EF09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,10 +18,21 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Backlog!$A$1:$AB$67</definedName>
   </definedNames>
-  <calcPr calcId="179021"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -425,6 +436,7 @@
       <sz val="9"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -770,8 +782,8 @@
   </sheetPr>
   <dimension ref="A1:L1017"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="L16" sqref="L16"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -780,8 +792,8 @@
     <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="94.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="35.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="106.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -1100,7 +1112,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:12" ht="24" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <f t="shared" si="0"/>
         <v>8</v>

</xml_diff>